<commit_message>
Updating the gallery Deleting the uploader name Slight modification to the sheet output
</commit_message>
<xml_diff>
--- a/PyProject/Treated_Sheet/Column_Sums.xlsx
+++ b/PyProject/Treated_Sheet/Column_Sums.xlsx
@@ -417,7 +417,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>12909</v>
+        <v>33470</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -425,7 +425,7 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>32324</v>
+        <v>71711</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -433,7 +433,7 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>22526</v>
+        <v>47137</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -441,7 +441,7 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>252</v>
+        <v>712</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -449,7 +449,7 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>438</v>
+        <v>1369</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -457,7 +457,7 @@
         <v>7</v>
       </c>
       <c r="B7">
-        <v>41</v>
+        <v>127</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -465,7 +465,7 @@
         <v>8</v>
       </c>
       <c r="B8">
-        <v>252</v>
+        <v>782</v>
       </c>
     </row>
   </sheetData>

</xml_diff>